<commit_message>
modal window without ajax
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_DIVYASRI.xlsx
+++ b/Wave 5_React_Tracker_DIVYASRI.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>React Basics (Architecture, Concepts, Lifecycle)</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>24/08/2016</t>
+  </si>
+  <si>
+    <t>25/08/2016</t>
+  </si>
+  <si>
+    <t>working in progress</t>
   </si>
 </sst>
 </file>
@@ -407,7 +413,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -562,6 +568,35 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
view and send messages
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_DIVYASRI.xlsx
+++ b/Wave 5_React_Tracker_DIVYASRI.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
   <si>
     <t>React Basics (Architecture, Concepts, Lifecycle)</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>working in progress</t>
+  </si>
+  <si>
+    <t>26/08/2016</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -597,6 +600,38 @@
         <v>20</v>
       </c>
     </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>